<commit_message>
Final tweaks to the Wildlife License SSPs
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Wildlife_License_Query_Results/artifacts/service_model/information_model/IEPD/documentation/Wildlife_License_Query_Results.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Wildlife_License_Query_Results/artifacts/service_model/information_model/IEPD/documentation/Wildlife_License_Query_Results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5740" yWindow="940" windowWidth="28900" windowHeight="16060"/>
+    <workbookView xWindow="4940" yWindow="1720" windowWidth="28900" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="eCitation" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="48">
   <si>
     <t>Description</t>
   </si>
@@ -79,6 +79,90 @@
   </si>
   <si>
     <t>Wildlife License Report (Information</t>
+  </si>
+  <si>
+    <t>Person</t>
+  </si>
+  <si>
+    <t>Contact/Mailing Address</t>
+  </si>
+  <si>
+    <t>Residence</t>
+  </si>
+  <si>
+    <t>Telephone Number</t>
+  </si>
+  <si>
+    <t>Query Results System</t>
+  </si>
+  <si>
+    <t>/wlq-res-doc:WildlifeLicenseQueryResults/wlq-res-ext:WildlifeLicenseReport/intel:SystemIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>System ID</t>
+  </si>
+  <si>
+    <t>System Name</t>
+  </si>
+  <si>
+    <t>/wlq-res-doc:WildlifeLicenseQueryResults/wlq-res-ext:WildlifeLicenseReport/intel:SystemIdentification/nc:SystemName</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Middle Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>Eye Color</t>
+  </si>
+  <si>
+    <t>Hair Color</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Height</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t>Height Units</t>
+  </si>
+  <si>
+    <t>Weight Units</t>
+  </si>
+  <si>
+    <t>Street</t>
+  </si>
+  <si>
+    <t>Secondary</t>
+  </si>
+  <si>
+    <t>Country Name</t>
+  </si>
+  <si>
+    <t>State Abbrv</t>
+  </si>
+  <si>
+    <t>City Name</t>
+  </si>
+  <si>
+    <t>Zip Code</t>
+  </si>
+  <si>
+    <t>Zip Code Extension</t>
+  </si>
+  <si>
+    <t>Full Telephone Number</t>
+  </si>
+  <si>
+    <t>DOB</t>
   </si>
 </sst>
 </file>
@@ -88,7 +172,7 @@
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -178,6 +262,12 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
@@ -289,7 +379,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="736">
+  <cellStyleXfs count="750">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
@@ -1026,8 +1116,22 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1062,20 +1166,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="736">
+  <cellStyles count="750">
     <cellStyle name="Accent1 - 20%" xfId="3"/>
     <cellStyle name="Accent1 - 40%" xfId="4"/>
     <cellStyle name="Accent1 - 60%" xfId="5"/>
@@ -1452,6 +1559,13 @@
     <cellStyle name="Followed Hyperlink" xfId="731" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="733" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="735" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="737" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="739" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="741" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="743" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="745" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="747" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="749" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
@@ -1807,6 +1921,13 @@
     <cellStyle name="Hyperlink" xfId="730" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="732" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="734" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="736" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="738" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="740" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="742" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="744" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="746" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="748" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal 3" xfId="24"/>
@@ -2110,11 +2231,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A12" sqref="A12:XFD12"/>
+      <selection pane="bottomLeft" activeCell="A35" sqref="A35:XFD37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2128,12 +2249,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="8" customFormat="1" ht="20" customHeight="1">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
     </row>
     <row r="2" spans="1:4" s="6" customFormat="1" ht="15">
       <c r="A2" s="9" t="s">
@@ -2214,38 +2335,198 @@
       </c>
     </row>
     <row r="11" spans="1:4" s="8" customFormat="1" ht="33" customHeight="1">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
     </row>
     <row r="12" spans="1:4" s="8" customFormat="1" ht="19" customHeight="1">
       <c r="A12" s="7" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
     </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="10"/>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="10"/>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="10"/>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="10"/>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" s="10"/>
-    </row>
-    <row r="18" spans="1:1">
-      <c r="A18" s="10"/>
+    <row r="13" spans="1:4" s="8" customFormat="1">
+      <c r="A13" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" s="8" customFormat="1">
+      <c r="A14" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" s="8" customFormat="1" ht="19" customHeight="1">
+      <c r="A15" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="1:4" s="8" customFormat="1" ht="14" customHeight="1">
+      <c r="A16" s="16" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="14" customHeight="1">
+      <c r="A17" s="10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" s="8" customFormat="1">
+      <c r="A24" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" s="8" customFormat="1" ht="19" customHeight="1">
+      <c r="A27" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" s="8" customFormat="1" ht="19" customHeight="1">
+      <c r="A35" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" s="8" customFormat="1" ht="19" customHeight="1">
+      <c r="A43" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B43" s="3"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="1" t="s">
+        <v>46</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Completed mapping sheet and final cleanup of SSP.
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Wildlife_License_Query_Results/artifacts/service_model/information_model/IEPD/documentation/Wildlife_License_Query_Results.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Wildlife_License_Query_Results/artifacts/service_model/information_model/IEPD/documentation/Wildlife_License_Query_Results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4940" yWindow="1720" windowWidth="28900" windowHeight="16060"/>
+    <workbookView xWindow="5160" yWindow="3060" windowWidth="28900" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="eCitation" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="72">
   <si>
     <t>Description</t>
   </si>
@@ -132,12 +132,6 @@
     <t>Weight</t>
   </si>
   <si>
-    <t>Height Units</t>
-  </si>
-  <si>
-    <t>Weight Units</t>
-  </si>
-  <si>
     <t>Street</t>
   </si>
   <si>
@@ -159,10 +153,95 @@
     <t>Zip Code Extension</t>
   </si>
   <si>
-    <t>Full Telephone Number</t>
-  </si>
-  <si>
-    <t>DOB</t>
+    <t>/wlq-res-doc:WildlifeLicenseQueryResults/wlq-res-ext:WildlifeLicenseReport/nc:Person/nc:PersonEyeColorText</t>
+  </si>
+  <si>
+    <t>/wlq-res-doc:WildlifeLicenseQueryResults/wlq-res-ext:WildlifeLicenseReport/nc:Person/nc:PersonName/nc:PersonGivenName</t>
+  </si>
+  <si>
+    <t>/wlq-res-doc:WildlifeLicenseQueryResults/wlq-res-ext:WildlifeLicenseReport/nc:Person/nc:PersonName/nc:PersonMiddleName</t>
+  </si>
+  <si>
+    <t>/wlq-res-doc:WildlifeLicenseQueryResults/wlq-res-ext:WildlifeLicenseReport/nc:Person/nc:PersonName/nc:PersonSurName</t>
+  </si>
+  <si>
+    <t>/wlq-res-doc:WildlifeLicenseQueryResults/wlq-res-ext:WildlifeLicenseReport/nc:Person/nc:PersonHairColorText</t>
+  </si>
+  <si>
+    <t>/wlq-res-doc:WildlifeLicenseQueryResults/wlq-res-ext:WildlifeLicenseReport/nc:Person/j:PersonSexCode</t>
+  </si>
+  <si>
+    <t>/wlq-res-doc:WildlifeLicenseQueryResults/wlq-res-ext:WildlifeLicenseReport/nc:Person/nc:PersonHeightMeasure/nc:MeasureValueText</t>
+  </si>
+  <si>
+    <t>Height Unit</t>
+  </si>
+  <si>
+    <t>Weight Unit</t>
+  </si>
+  <si>
+    <t>/wlq-res-doc:WildlifeLicenseQueryResults/wlq-res-ext:WildlifeLicenseReport/nc:Person/nc:PersonHeightMeasure/nc:LengthUnitCode</t>
+  </si>
+  <si>
+    <t>/wlq-res-doc:WildlifeLicenseQueryResults/wlq-res-ext:WildlifeLicenseReport/nc:Person/nc:PersonWeightMeasure/nc:MeasureValueText</t>
+  </si>
+  <si>
+    <t>/wlq-res-doc:WildlifeLicenseQueryResults/wlq-res-ext:WildlifeLicenseReport/nc:Person/nc:PersonWeightMeasure/nc:WeightUnitCode</t>
+  </si>
+  <si>
+    <t>Full Street Address</t>
+  </si>
+  <si>
+    <t>Unit, PO Box, etc.</t>
+  </si>
+  <si>
+    <t>/wlq-res-doc:WildlifeLicenseQueryResults/wlq-res-ext:WildlifeLicenseReport/nc:Location[@structures:id=
+../nc:PersonResidenceAssociation/nc:Location/@structures:ref]/nc:Address/nc:LocationStreet/nc:StreetFullText</t>
+  </si>
+  <si>
+    <t>/wlq-res-doc:WildlifeLicenseQueryResults/wlq-res-ext:WildlifeLicenseReport/nc:Location[@structures:id=
+../nc:PersonResidenceAssociation/nc:Location/@structures:ref]/nc:Address/nc:AddressSecondaryUnitText</t>
+  </si>
+  <si>
+    <t>/wlq-res-doc:WildlifeLicenseQueryResults/wlq-res-ext:WildlifeLicenseReport/nc:Location[@structures:id=
+../nc:PersonResidenceAssociation/nc:Location/@structures:ref]/nc:Address/nc:LocationCityName</t>
+  </si>
+  <si>
+    <t>/wlq-res-doc:WildlifeLicenseQueryResults/wlq-res-ext:WildlifeLicenseReport/nc:Location[@structures:id=
+../nc:PersonResidenceAssociation/nc:Location/@structures:ref]/nc:Address/j:LocationStateNCICLISCode</t>
+  </si>
+  <si>
+    <t>/wlq-res-doc:WildlifeLicenseQueryResults/wlq-res-ext:WildlifeLicenseReport/nc:Location[@structures:id=
+../nc:PersonResidenceAssociation/nc:Location/@structures:ref]/nc:Address/nc:LocationCountryName</t>
+  </si>
+  <si>
+    <t>/wlq-res-doc:WildlifeLicenseQueryResults/wlq-res-ext:WildlifeLicenseReport/nc:Location[@structures:id=
+../nc:PersonResidenceAssociation/nc:Location/@structures:ref]/nc:Address/nc:LocationPostalCode</t>
+  </si>
+  <si>
+    <t>/wlq-res-doc:WildlifeLicenseQueryResults/wlq-res-ext:WildlifeLicenseReport/nc:Location[@structures:id=
+../nc:PersonResidenceAssociation/nc:Location/@structures:ref]/nc:Address/nc:LocationPostalExtensionCode</t>
+  </si>
+  <si>
+    <t>/wlq-res-doc:WildlifeLicenseQueryResults/wlq-res-ext:WildlifeLicenseReport/nc:ContactInformation/nc:ContactMailingAddress[@structures:id=../../nc:ContactInformationAssociation/nc:ContactInformation/@structures:ref]/nc:LocationStreet/nc:StreetFullText</t>
+  </si>
+  <si>
+    <t>/wlq-res-doc:WildlifeLicenseQueryResults/wlq-res-ext:WildlifeLicenseReport/nc:ContactInformation/nc:ContactMailingAddress[@structures:id=../../nc:ContactInformationAssociation/nc:ContactInformation/@structures:ref]/nc:AddressSecondaryUnitText</t>
+  </si>
+  <si>
+    <t>/wlq-res-doc:WildlifeLicenseQueryResults/wlq-res-ext:WildlifeLicenseReport/nc:ContactInformation/nc:ContactMailingAddress[@structures:id=../../nc:ContactInformationAssociation/nc:ContactInformation/@structures:ref]/nc:LocationCityName</t>
+  </si>
+  <si>
+    <t>/wlq-res-doc:WildlifeLicenseQueryResults/wlq-res-ext:WildlifeLicenseReport/nc:ContactInformation/nc:ContactMailingAddress[@structures:id=../../nc:ContactInformationAssociation/nc:ContactInformation/@structures:ref]/j:LocationStateNCICLISCode</t>
+  </si>
+  <si>
+    <t>/wlq-res-doc:WildlifeLicenseQueryResults/wlq-res-ext:WildlifeLicenseReport/nc:ContactInformation/nc:ContactMailingAddress[@structures:id=../../nc:ContactInformationAssociation/nc:ContactInformation/@structures:ref]/nc:LocationCountryName</t>
+  </si>
+  <si>
+    <t>/wlq-res-doc:WildlifeLicenseQueryResults/wlq-res-ext:WildlifeLicenseReport/nc:ContactInformation/nc:ContactMailingAddress[@structures:id=../../nc:ContactInformationAssociation/nc:ContactInformation/@structures:ref]/nc:LocationPostalCode</t>
+  </si>
+  <si>
+    <t>/wlq-res-doc:WildlifeLicenseQueryResults/wlq-res-ext:WildlifeLicenseReport/nc:ContactInformation/nc:ContactMailingAddress[@structures:id=../../nc:ContactInformationAssociation/nc:ContactInformation/@structures:ref]/nc:LocationPostalExtensionCode</t>
   </si>
 </sst>
 </file>
@@ -172,7 +251,7 @@
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -262,12 +341,6 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
@@ -379,7 +452,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="750">
+  <cellStyleXfs count="788">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
@@ -1130,8 +1203,46 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1178,11 +1289,8 @@
     <xf numFmtId="0" fontId="13" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="750">
+  <cellStyles count="788">
     <cellStyle name="Accent1 - 20%" xfId="3"/>
     <cellStyle name="Accent1 - 40%" xfId="4"/>
     <cellStyle name="Accent1 - 60%" xfId="5"/>
@@ -1566,6 +1674,25 @@
     <cellStyle name="Followed Hyperlink" xfId="745" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="747" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="749" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="751" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="753" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="755" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="757" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="759" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="761" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="763" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="765" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="767" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="769" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="771" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="773" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="775" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="777" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="779" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="781" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="783" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="785" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="787" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
@@ -1928,6 +2055,25 @@
     <cellStyle name="Hyperlink" xfId="744" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="746" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="748" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="750" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="752" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="754" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="756" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="758" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="760" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="762" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="764" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="766" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="768" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="770" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="772" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="774" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="776" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="778" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="780" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="782" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="784" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="786" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal 3" xfId="24"/>
@@ -2231,11 +2377,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D44"/>
+  <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A35" sqref="A35:XFD37"/>
+      <selection pane="bottomLeft" activeCell="A43" sqref="A43:XFD43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2374,159 +2520,227 @@
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
     </row>
-    <row r="16" spans="1:4" s="8" customFormat="1" ht="14" customHeight="1">
-      <c r="A16" s="16" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="14" customHeight="1">
+    <row r="16" spans="1:4" ht="14" customHeight="1">
+      <c r="A16" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" s="10" t="s">
-        <v>29</v>
+        <v>30</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="10" t="s">
-        <v>30</v>
+        <v>31</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="10" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="10" t="s">
-        <v>32</v>
+        <v>33</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="10" t="s">
-        <v>33</v>
+        <v>34</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="10" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="1" t="s">
+      <c r="A22" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" s="8" customFormat="1">
-      <c r="A24" s="8" t="s">
-        <v>37</v>
+      <c r="D22" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" s="8" customFormat="1">
+      <c r="A23" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" s="8" customFormat="1" ht="19" customHeight="1">
+      <c r="A26" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+    </row>
+    <row r="27" spans="1:4" ht="42">
+      <c r="A27" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="42">
+      <c r="A28" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" s="8" customFormat="1" ht="19" customHeight="1">
-      <c r="A27" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" s="1" t="s">
+      <c r="B28" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="42">
+      <c r="A29" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="42">
+      <c r="A30" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="42">
+      <c r="A31" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29" s="1" t="s">
+      <c r="D31" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="42">
+      <c r="A32" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="42">
+      <c r="A33" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" s="8" customFormat="1" ht="19" customHeight="1">
+      <c r="A34" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+    </row>
+    <row r="35" spans="1:4" ht="28">
+      <c r="A35" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="28">
+      <c r="A36" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="28">
+      <c r="A37" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="28">
+      <c r="A38" s="8" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" s="1" t="s">
+      <c r="D38" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="28">
+      <c r="A39" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="28">
+      <c r="A40" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="28">
+      <c r="A41" s="8" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="A31" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
-      <c r="A32" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="A33" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="A34" s="8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" s="8" customFormat="1" ht="19" customHeight="1">
-      <c r="A35" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
-    </row>
-    <row r="36" spans="1:4">
-      <c r="A36" s="8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
-      <c r="A37" s="8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="A38" s="8" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="A39" s="8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4">
-      <c r="A40" s="8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4">
-      <c r="A41" s="8" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4">
-      <c r="A42" s="8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" s="8" customFormat="1" ht="19" customHeight="1">
-      <c r="A43" s="7" t="s">
+      <c r="D41" s="8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" s="8" customFormat="1" ht="19" customHeight="1">
+      <c r="A42" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B43" s="3"/>
-      <c r="C43" s="3"/>
-      <c r="D43" s="3"/>
-    </row>
-    <row r="44" spans="1:4">
-      <c r="A44" s="1" t="s">
-        <v>46</v>
-      </c>
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Added DOB to IEPD
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Wildlife_License_Query_Results/artifacts/service_model/information_model/IEPD/documentation/Wildlife_License_Query_Results.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Wildlife_License_Query_Results/artifacts/service_model/information_model/IEPD/documentation/Wildlife_License_Query_Results.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="84">
   <si>
     <t>Description</t>
   </si>
@@ -280,6 +280,12 @@
   </si>
   <si>
     <t>/wlq-res-doc:WildlifeLicenseQueryResults/wlq-res-ext:WildlifeLicenseReport/nc:ContactInformation[@structures:id=../nc:ContactInformationAssociation/nc:ContactInformation/@structures:ref]/nc:ContactMailingAddress/nc:LocationCountryName</t>
+  </si>
+  <si>
+    <t>DOB</t>
+  </si>
+  <si>
+    <t>/wlq-res-doc:WildlifeLicenseQueryResults/wlq-res-ext:WildlifeLicenseReport/nc:Person/nc:PersonBirthDate/nc:Date</t>
   </si>
 </sst>
 </file>
@@ -490,7 +496,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="802">
+  <cellStyleXfs count="804">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
@@ -517,6 +523,8 @@
     <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1342,7 +1350,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="802">
+  <cellStyles count="804">
     <cellStyle name="Accent1 - 20%" xfId="3"/>
     <cellStyle name="Accent1 - 40%" xfId="4"/>
     <cellStyle name="Accent1 - 60%" xfId="5"/>
@@ -1752,6 +1760,7 @@
     <cellStyle name="Followed Hyperlink" xfId="797" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="799" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="801" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="803" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
@@ -2140,6 +2149,7 @@
     <cellStyle name="Hyperlink" xfId="796" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="798" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="800" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="802" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal 3" xfId="24"/>
@@ -2443,11 +2453,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D51"/>
+  <dimension ref="A1:D52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C28" sqref="C28"/>
+      <pane ySplit="2" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2586,297 +2596,305 @@
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
     </row>
-    <row r="16" spans="1:4" ht="14" customHeight="1">
-      <c r="A16" s="10" t="s">
+    <row r="16" spans="1:4" s="8" customFormat="1" ht="19" customHeight="1">
+      <c r="A16" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="14" customHeight="1">
+      <c r="A17" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D22" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="1" t="s">
+    <row r="23" spans="1:4">
+      <c r="A23" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="D23" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:4" s="8" customFormat="1">
-      <c r="A23" s="8" t="s">
+    <row r="24" spans="1:4" s="8" customFormat="1">
+      <c r="A24" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="D23" s="8" t="s">
+      <c r="D24" s="8" t="s">
         <v>52</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D26" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="1:4" s="8" customFormat="1" ht="19" customHeight="1">
-      <c r="A26" s="7" t="s">
+    <row r="27" spans="1:4" s="8" customFormat="1" ht="19" customHeight="1">
+      <c r="A27" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-    </row>
-    <row r="27" spans="1:4" ht="42">
-      <c r="A27" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D27" s="8" t="s">
-        <v>77</v>
-      </c>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
     </row>
     <row r="28" spans="1:4" ht="42">
       <c r="A28" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="42">
       <c r="A29" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>56</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="42">
       <c r="A30" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="42">
       <c r="A31" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="42">
       <c r="A32" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="42">
+      <c r="A33" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D32" s="8" t="s">
+      <c r="D33" s="8" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="42">
-      <c r="A33" s="8" t="s">
+    <row r="34" spans="1:4" ht="42">
+      <c r="A34" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="D33" s="8" t="s">
+      <c r="D34" s="8" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="34" spans="1:4" s="8" customFormat="1" ht="19" customHeight="1">
-      <c r="A34" s="7" t="s">
+    <row r="35" spans="1:4" s="8" customFormat="1" ht="19" customHeight="1">
+      <c r="A35" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
-    </row>
-    <row r="35" spans="1:4" s="8" customFormat="1" ht="56">
-      <c r="A35" s="8" t="s">
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+    </row>
+    <row r="36" spans="1:4" s="8" customFormat="1" ht="56">
+      <c r="A36" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="D35" s="8" t="s">
+      <c r="D36" s="8" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="36" spans="1:4" s="8" customFormat="1" ht="19" customHeight="1">
-      <c r="A36" s="7" t="s">
+    <row r="37" spans="1:4" s="8" customFormat="1" ht="19" customHeight="1">
+      <c r="A37" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="B36" s="3"/>
-      <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
-    </row>
-    <row r="37" spans="1:4" ht="28">
-      <c r="A37" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="D37" s="8" t="s">
-        <v>57</v>
-      </c>
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
     </row>
     <row r="38" spans="1:4" ht="28">
       <c r="A38" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="28">
       <c r="A39" s="8" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="28">
       <c r="A40" s="8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="28">
       <c r="A41" s="8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="28">
       <c r="A42" s="8" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="28">
       <c r="A43" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D43" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="28">
+      <c r="A44" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="D43" s="8" t="s">
+      <c r="D44" s="8" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="44" spans="1:4" s="8" customFormat="1" ht="19" customHeight="1">
-      <c r="A44" s="7" t="s">
+    <row r="45" spans="1:4" s="8" customFormat="1" ht="19" customHeight="1">
+      <c r="A45" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="B44" s="3"/>
-      <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
-    </row>
-    <row r="45" spans="1:4" s="8" customFormat="1" ht="28">
-      <c r="A45" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="D45" s="8" t="s">
-        <v>66</v>
-      </c>
+      <c r="B45" s="3"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
     </row>
     <row r="46" spans="1:4" s="8" customFormat="1" ht="28">
       <c r="A46" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="47" spans="1:4" s="8" customFormat="1" ht="28">
       <c r="A47" s="8" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="48" spans="1:4" s="8" customFormat="1" ht="28">
       <c r="A48" s="8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="49" spans="1:4" s="8" customFormat="1" ht="28">
       <c r="A49" s="8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="50" spans="1:4" s="8" customFormat="1" ht="28">
       <c r="A50" s="8" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="51" spans="1:4" s="8" customFormat="1" ht="28">
       <c r="A51" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D51" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" s="8" customFormat="1" ht="28">
+      <c r="A52" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="D51" s="8" t="s">
+      <c r="D52" s="8" t="s">
         <v>72</v>
       </c>
     </row>

</xml_diff>